<commit_message>
Add budget grid search files (1)
</commit_message>
<xml_diff>
--- a/Outputs/1. Budget/Grid Search/Output Files/100000/Output_0_0.xlsx
+++ b/Outputs/1. Budget/Grid Search/Output Files/100000/Output_0_0.xlsx
@@ -480,8 +480,10 @@
           <t>Required Level of Met Demand</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -511,7 +513,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10144950.40989403</v>
+        <v>10247649.0453073</v>
       </c>
     </row>
     <row r="8">
@@ -521,7 +523,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27457249.52289559</v>
+        <v>27559948.15830886</v>
       </c>
     </row>
     <row r="9">
@@ -541,7 +543,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1803024.648971332</v>
+        <v>1775725.279432752</v>
       </c>
     </row>
     <row r="11">
@@ -7979,22 +7981,22 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L2" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O2" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -8061,7 +8063,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M3" t="n">
         <v>142.1340339220183</v>
@@ -8140,10 +8142,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -8216,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L5" t="n">
         <v>235.7664149699872</v>
@@ -8225,10 +8227,10 @@
         <v>230.3462332272727</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O5" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
         <v>231.2329957552695</v>
@@ -8295,16 +8297,16 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L6" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O6" t="n">
         <v>142.5962444444444</v>
@@ -8383,7 +8385,7 @@
         <v>138.9257839476051</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -8456,19 +8458,19 @@
         <v>220.0898510449805</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O8" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -8535,7 +8537,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -8544,13 +8546,13 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
         <v>133.9744074143302</v>
       </c>
       <c r="Q9" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -8614,16 +8616,16 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M10" t="n">
         <v>138.9257839476051</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -8696,16 +8698,16 @@
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P11" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
@@ -8769,13 +8771,13 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>138.5543797798742</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -8787,7 +8789,7 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
@@ -8854,10 +8856,10 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N13" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
@@ -8927,19 +8929,19 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N14" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
         <v>231.2329957552695</v>
@@ -9006,7 +9008,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L15" t="n">
         <v>138.5543797798742</v>
@@ -9015,13 +9017,13 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P15" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
         <v>139.9817740860215</v>
@@ -9088,16 +9090,16 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -9164,22 +9166,22 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -9243,10 +9245,10 @@
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
         <v>142.1340339220183</v>
@@ -9325,16 +9327,16 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M19" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O19" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
@@ -9480,22 +9482,22 @@
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L21" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q21" t="n">
         <v>139.9817740860215</v>
@@ -9562,16 +9564,16 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N22" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
@@ -9644,7 +9646,7 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N23" t="n">
         <v>229.4130635965909</v>
@@ -9720,10 +9722,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -9799,13 +9801,13 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O25" t="n">
         <v>138.4565384518428</v>
@@ -9875,19 +9877,19 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M26" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
         <v>229.4130635965909</v>
       </c>
       <c r="O26" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P26" t="n">
         <v>231.2329957552695</v>
@@ -9954,16 +9956,16 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
@@ -10036,10 +10038,10 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N28" t="n">
         <v>127.6855444652332</v>
@@ -10118,13 +10120,13 @@
         <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O29" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P29" t="n">
         <v>231.2329957552695</v>
@@ -10191,16 +10193,16 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
         <v>138.5543797798742</v>
       </c>
       <c r="M30" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O30" t="n">
         <v>142.5962444444444</v>
@@ -10209,7 +10211,7 @@
         <v>0</v>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R30" t="n">
         <v>0</v>
@@ -10276,7 +10278,7 @@
         <v>134.8846762812383</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N31" t="n">
         <v>127.6855444652332</v>
@@ -10355,16 +10357,16 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O32" t="n">
         <v>230.0982114216867</v>
       </c>
       <c r="P32" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -10437,16 +10439,16 @@
         <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O33" t="n">
         <v>142.5962444444444</v>
       </c>
       <c r="P33" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>0</v>
@@ -10516,10 +10518,10 @@
         <v>138.9257839476051</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P34" t="n">
         <v>0</v>
@@ -10592,7 +10594,7 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M35" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -10665,22 +10667,22 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
       </c>
       <c r="O36" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P36" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
@@ -10750,13 +10752,13 @@
         <v>134.8846762812383</v>
       </c>
       <c r="M37" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P37" t="n">
         <v>0</v>
@@ -10829,16 +10831,16 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M38" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O38" t="n">
         <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q38" t="n">
         <v>0</v>
@@ -10902,7 +10904,7 @@
         <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L39" t="n">
         <v>138.5543797798742</v>
@@ -10914,13 +10916,13 @@
         <v>131.3417120833333</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P39" t="n">
         <v>133.9744074143302</v>
       </c>
       <c r="Q39" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R39" t="n">
         <v>0</v>
@@ -10990,7 +10992,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O40" t="n">
         <v>138.4565384518428</v>
@@ -11060,13 +11062,13 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L41" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M41" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N41" t="n">
         <v>0</v>
@@ -11139,16 +11141,16 @@
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L42" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N42" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
         <v>142.5962444444444</v>
@@ -11224,13 +11226,13 @@
         <v>134.8846762812383</v>
       </c>
       <c r="M43" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N43" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P43" t="n">
         <v>0</v>
@@ -11300,16 +11302,16 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
         <v>229.4130635965909</v>
       </c>
       <c r="O44" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P44" t="n">
         <v>0</v>
@@ -11376,22 +11378,22 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L45" t="n">
         <v>138.5543797798742</v>
       </c>
       <c r="M45" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
         <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q45" t="n">
         <v>139.9817740860215</v>
@@ -11458,13 +11460,13 @@
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -22571,22 +22573,22 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K2" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P2" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>222.3056898744495</v>
@@ -22653,7 +22655,7 @@
         <v>137.841438974359</v>
       </c>
       <c r="L3" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -22732,10 +22734,10 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N4" t="n">
         <v>127.6855444652332</v>
@@ -22808,7 +22810,7 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K5" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -22817,10 +22819,10 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -22887,16 +22889,16 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K6" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M6" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -22975,7 +22977,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>138.4565384518428</v>
@@ -23048,19 +23050,19 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q8" t="n">
         <v>222.3056898744495</v>
@@ -23127,7 +23129,7 @@
         <v>137.841438974359</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M9" t="n">
         <v>142.1340339220183</v>
@@ -23136,13 +23138,13 @@
         <v>131.3417120833333</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R9" t="n">
         <v>145.679503963964</v>
@@ -23206,16 +23208,16 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L10" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
         <v>137.7280040491476</v>
@@ -23288,16 +23290,16 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N11" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q11" t="n">
         <v>222.3056898744495</v>
@@ -23361,13 +23363,13 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
         <v>131.3417120833333</v>
@@ -23379,7 +23381,7 @@
         <v>133.9744074143302</v>
       </c>
       <c r="Q12" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
         <v>145.679503963964</v>
@@ -23446,10 +23448,10 @@
         <v>134.8846762812383</v>
       </c>
       <c r="M13" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O13" t="n">
         <v>138.4565384518428</v>
@@ -23519,19 +23521,19 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -23598,7 +23600,7 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K15" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -23607,13 +23609,13 @@
         <v>142.1340339220183</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O15" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
@@ -23680,16 +23682,16 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L16" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
         <v>138.9257839476051</v>
       </c>
       <c r="N16" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
         <v>137.7280040491476</v>
@@ -23756,22 +23758,22 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L17" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O17" t="n">
         <v>230.0982114216867</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q17" t="n">
         <v>222.3056898744495</v>
@@ -23835,10 +23837,10 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
@@ -23917,16 +23919,16 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L19" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N19" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P19" t="n">
         <v>137.7280040491476</v>
@@ -24072,22 +24074,22 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K21" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O21" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
@@ -24154,16 +24156,16 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L22" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P22" t="n">
         <v>137.7280040491476</v>
@@ -24236,7 +24238,7 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
@@ -24312,10 +24314,10 @@
         <v>137.841438974359</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N24" t="n">
         <v>131.3417120833333</v>
@@ -24391,13 +24393,13 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M25" t="n">
         <v>138.9257839476051</v>
       </c>
       <c r="N25" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -24467,19 +24469,19 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L26" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
@@ -24546,16 +24548,16 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M27" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O27" t="n">
         <v>142.5962444444444</v>
@@ -24628,10 +24630,10 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M28" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -24710,13 +24712,13 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N29" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P29" t="n">
         <v>0</v>
@@ -24783,16 +24785,16 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N30" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -24801,7 +24803,7 @@
         <v>133.9744074143302</v>
       </c>
       <c r="Q30" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R30" t="n">
         <v>145.679503963964</v>
@@ -24868,7 +24870,7 @@
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -24947,16 +24949,16 @@
         <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q32" t="n">
         <v>222.3056898744495</v>
@@ -25029,16 +25031,16 @@
         <v>142.1340339220183</v>
       </c>
       <c r="N33" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R33" t="n">
         <v>145.679503963964</v>
@@ -25108,10 +25110,10 @@
         <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P34" t="n">
         <v>137.7280040491476</v>
@@ -25184,7 +25186,7 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N35" t="n">
         <v>229.4130635965909</v>
@@ -25257,22 +25259,22 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M36" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
         <v>131.3417120833333</v>
       </c>
       <c r="O36" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q36" t="n">
         <v>139.9817740860215</v>
@@ -25342,13 +25344,13 @@
         <v>0</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N37" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P37" t="n">
         <v>137.7280040491476</v>
@@ -25421,16 +25423,16 @@
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N38" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O38" t="n">
         <v>230.0982114216867</v>
       </c>
       <c r="P38" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
         <v>222.3056898744495</v>
@@ -25494,7 +25496,7 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K39" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L39" t="n">
         <v>0</v>
@@ -25506,13 +25508,13 @@
         <v>0</v>
       </c>
       <c r="O39" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P39" t="n">
         <v>0</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R39" t="n">
         <v>145.679503963964</v>
@@ -25582,7 +25584,7 @@
         <v>138.9257839476051</v>
       </c>
       <c r="N40" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
         <v>0</v>
@@ -25652,13 +25654,13 @@
         <v>181.0459045266863</v>
       </c>
       <c r="K41" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
         <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N41" t="n">
         <v>229.4130635965909</v>
@@ -25731,16 +25733,16 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K42" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M42" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -25816,13 +25818,13 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P43" t="n">
         <v>137.7280040491476</v>
@@ -25892,16 +25894,16 @@
         <v>220.0898510449805</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P44" t="n">
         <v>231.2329957552695</v>
@@ -25968,22 +25970,22 @@
         <v>126.8376266666667</v>
       </c>
       <c r="K45" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L45" t="n">
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N45" t="n">
         <v>131.3417120833333</v>
       </c>
       <c r="O45" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="n">
         <v>0</v>
@@ -26050,13 +26052,13 @@
         <v>129.0132581705354</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N46" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O46" t="n">
         <v>138.4565384518428</v>
@@ -26123,7 +26125,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>123023.5991224671</v>
+        <v>216665.3565283203</v>
       </c>
     </row>
     <row r="3">
@@ -26131,7 +26133,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>181881.8933680103</v>
+        <v>238046.7615399077</v>
       </c>
     </row>
     <row r="4">
@@ -26139,7 +26141,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>141945.7613208857</v>
+        <v>160164.1557457211</v>
       </c>
     </row>
     <row r="5">
@@ -26147,7 +26149,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>131408.5068047156</v>
+        <v>142297.6890580523</v>
       </c>
     </row>
     <row r="6">
@@ -26155,7 +26157,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>200075.2934582162</v>
+        <v>155459.2308154412</v>
       </c>
     </row>
     <row r="7">
@@ -26163,7 +26165,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>189946.2638835197</v>
+        <v>41901.84325569165</v>
       </c>
     </row>
     <row r="8">
@@ -26171,7 +26173,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>117032.1929093238</v>
+        <v>117531.0065629728</v>
       </c>
     </row>
     <row r="9">
@@ -26179,7 +26181,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>158673.6189354638</v>
+        <v>169631.4053910703</v>
       </c>
     </row>
     <row r="10">
@@ -26187,7 +26189,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>200889.5901179787</v>
+        <v>138886.4814571525</v>
       </c>
     </row>
     <row r="11">
@@ -26195,7 +26197,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>179672.6893765823</v>
+        <v>152682.9235066417</v>
       </c>
     </row>
     <row r="12">
@@ -26203,7 +26205,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>164507.2879465382</v>
+        <v>196936.9755371677</v>
       </c>
     </row>
     <row r="13">
@@ -26211,7 +26213,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>137537.518255763</v>
+        <v>101470.8883970057</v>
       </c>
     </row>
     <row r="14">
@@ -26219,7 +26221,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>121644.8505094455</v>
+        <v>169510.2376286328</v>
       </c>
     </row>
     <row r="15">
@@ -26227,7 +26229,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>144432.2279852762</v>
+        <v>138408.3194632264</v>
       </c>
     </row>
     <row r="16">
@@ -26235,7 +26237,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>139600.4989163581</v>
+        <v>120789.4732342538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add budget outputs with UD penalty
</commit_message>
<xml_diff>
--- a/Outputs/1. Budget/Grid Search/Output Files/100000/Output_0_0.xlsx
+++ b/Outputs/1. Budget/Grid Search/Output Files/100000/Output_0_0.xlsx
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-91989.55041322313</v>
+        <v>-218750.5042824882</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10247649.0453073</v>
+        <v>5413711.842050619</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27559948.15830886</v>
+        <v>22726010.95505212</v>
       </c>
     </row>
     <row r="9">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1775725.279432752</v>
+        <v>4350924.71095404</v>
       </c>
     </row>
     <row r="11">
@@ -7978,7 +7978,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K2" t="n">
         <v>220.0898510449805</v>
@@ -7993,16 +7993,16 @@
         <v>229.4130635965909</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P2" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -8054,13 +8054,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L3" t="n">
         <v>138.5543797798742</v>
@@ -8078,10 +8078,10 @@
         <v>133.9744074143302</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -8136,28 +8136,28 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O4" t="n">
         <v>138.4565384518428</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -8215,7 +8215,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K5" t="n">
         <v>220.0898510449805</v>
@@ -8230,16 +8230,16 @@
         <v>229.4130635965909</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P5" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -8291,16 +8291,16 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K6" t="n">
         <v>137.841438974359</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M6" t="n">
         <v>142.1340339220183</v>
@@ -8318,7 +8318,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -8373,10 +8373,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L7" t="n">
         <v>134.8846762812383</v>
@@ -8388,13 +8388,13 @@
         <v>127.6855444652332</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -8452,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K8" t="n">
         <v>220.0898510449805</v>
@@ -8467,16 +8467,16 @@
         <v>229.4130635965909</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -8528,34 +8528,34 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P9" t="n">
         <v>133.9744074143302</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -8610,10 +8610,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L10" t="n">
         <v>134.8846762812383</v>
@@ -8628,10 +8628,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -8689,16 +8689,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K11" t="n">
         <v>220.0898510449805</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N11" t="n">
         <v>229.4130635965909</v>
@@ -8707,13 +8707,13 @@
         <v>230.0982114216867</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -8765,13 +8765,13 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L12" t="n">
         <v>138.5543797798742</v>
@@ -8780,19 +8780,19 @@
         <v>142.1340339220183</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O12" t="n">
         <v>142.5962444444444</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q12" t="n">
         <v>139.9817740860215</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
@@ -8847,28 +8847,28 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M13" t="n">
         <v>138.9257839476051</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R13" t="n">
         <v>0</v>
@@ -8926,10 +8926,10 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L14" t="n">
         <v>235.7664149699872</v>
@@ -8938,19 +8938,19 @@
         <v>230.3462332272727</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P14" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -9002,10 +9002,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K15" t="n">
         <v>137.841438974359</v>
@@ -9014,22 +9014,22 @@
         <v>138.5543797798742</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O15" t="n">
         <v>142.5962444444444</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q15" t="n">
         <v>139.9817740860215</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -9084,16 +9084,16 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L16" t="n">
         <v>134.8846762812383</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N16" t="n">
         <v>127.6855444652332</v>
@@ -9102,10 +9102,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -9163,31 +9163,31 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -9239,25 +9239,25 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M18" t="n">
         <v>142.1340339220183</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P18" t="n">
         <v>133.9744074143302</v>
@@ -9266,7 +9266,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -9321,28 +9321,28 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L19" t="n">
         <v>134.8846762812383</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N19" t="n">
         <v>127.6855444652332</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
@@ -9400,31 +9400,31 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L20" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O20" t="n">
         <v>230.0982114216867</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -9476,22 +9476,22 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K21" t="n">
         <v>137.841438974359</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O21" t="n">
         <v>142.5962444444444</v>
@@ -9503,7 +9503,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -9558,10 +9558,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L22" t="n">
         <v>134.8846762812383</v>
@@ -9570,16 +9570,16 @@
         <v>138.9257839476051</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R22" t="n">
         <v>0</v>
@@ -9637,7 +9637,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K23" t="n">
         <v>220.0898510449805</v>
@@ -9652,16 +9652,16 @@
         <v>229.4130635965909</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -9713,22 +9713,22 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O24" t="n">
         <v>142.5962444444444</v>
@@ -9740,7 +9740,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -9795,16 +9795,16 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N25" t="n">
         <v>127.6855444652332</v>
@@ -9813,10 +9813,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R25" t="n">
         <v>0</v>
@@ -9874,31 +9874,31 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L26" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N26" t="n">
         <v>229.4130635965909</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P26" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
@@ -9950,16 +9950,16 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M27" t="n">
         <v>142.1340339220183</v>
@@ -9968,16 +9968,16 @@
         <v>131.3417120833333</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q27" t="n">
         <v>139.9817740860215</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
@@ -10032,13 +10032,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M28" t="n">
         <v>138.9257839476051</v>
@@ -10047,13 +10047,13 @@
         <v>127.6855444652332</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q28" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R28" t="n">
         <v>0</v>
@@ -10111,31 +10111,31 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K29" t="n">
         <v>220.0898510449805</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N29" t="n">
         <v>229.4130635965909</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P29" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
@@ -10187,19 +10187,19 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L30" t="n">
         <v>138.5543797798742</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N30" t="n">
         <v>131.3417120833333</v>
@@ -10208,13 +10208,13 @@
         <v>142.5962444444444</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q30" t="n">
         <v>139.9817740860215</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
@@ -10269,10 +10269,10 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L31" t="n">
         <v>134.8846762812383</v>
@@ -10284,13 +10284,13 @@
         <v>127.6855444652332</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R31" t="n">
         <v>0</v>
@@ -10348,7 +10348,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K32" t="n">
         <v>220.0898510449805</v>
@@ -10366,13 +10366,13 @@
         <v>230.0982114216867</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -10424,19 +10424,19 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N33" t="n">
         <v>131.3417120833333</v>
@@ -10445,13 +10445,13 @@
         <v>142.5962444444444</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
@@ -10506,13 +10506,13 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M34" t="n">
         <v>138.9257839476051</v>
@@ -10524,10 +10524,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P34" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R34" t="n">
         <v>0</v>
@@ -10585,7 +10585,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K35" t="n">
         <v>220.0898510449805</v>
@@ -10594,22 +10594,22 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R35" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S35" t="n">
         <v>0</v>
@@ -10661,34 +10661,34 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>137.841438974359</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M36" t="n">
         <v>142.1340339220183</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O36" t="n">
         <v>142.5962444444444</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
@@ -10743,16 +10743,16 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L37" t="n">
         <v>134.8846762812383</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N37" t="n">
         <v>127.6855444652332</v>
@@ -10761,10 +10761,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R37" t="n">
         <v>0</v>
@@ -10822,31 +10822,31 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L38" t="n">
         <v>235.7664149699872</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N38" t="n">
         <v>229.4130635965909</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>230.0982114216867</v>
       </c>
       <c r="P38" t="n">
         <v>231.2329957552695</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S38" t="n">
         <v>0</v>
@@ -10898,10 +10898,10 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K39" t="n">
         <v>137.841438974359</v>
@@ -10922,10 +10922,10 @@
         <v>133.9744074143302</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S39" t="n">
         <v>0</v>
@@ -10980,16 +10980,16 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N40" t="n">
         <v>127.6855444652332</v>
@@ -10998,10 +10998,10 @@
         <v>138.4565384518428</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R40" t="n">
         <v>0</v>
@@ -11059,7 +11059,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K41" t="n">
         <v>220.0898510449805</v>
@@ -11068,22 +11068,22 @@
         <v>235.7664149699872</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N41" t="n">
-        <v>0</v>
+        <v>229.4130635965909</v>
       </c>
       <c r="O41" t="n">
         <v>230.0982114216867</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R41" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S41" t="n">
         <v>0</v>
@@ -11135,34 +11135,34 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K42" t="n">
         <v>137.841438974359</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>138.5543797798742</v>
       </c>
       <c r="M42" t="n">
         <v>142.1340339220183</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O42" t="n">
         <v>142.5962444444444</v>
       </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q42" t="n">
-        <v>0</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R42" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S42" t="n">
         <v>0</v>
@@ -11217,10 +11217,10 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L43" t="n">
         <v>134.8846762812383</v>
@@ -11229,16 +11229,16 @@
         <v>138.9257839476051</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>127.6855444652332</v>
       </c>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q43" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R43" t="n">
         <v>0</v>
@@ -11296,16 +11296,16 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>169.0966151720738</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>220.0898510449805</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>235.7664149699872</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>230.3462332272727</v>
       </c>
       <c r="N44" t="n">
         <v>229.4130635965909</v>
@@ -11314,13 +11314,13 @@
         <v>230.0982114216867</v>
       </c>
       <c r="P44" t="n">
-        <v>0</v>
+        <v>231.2329957552695</v>
       </c>
       <c r="Q44" t="n">
-        <v>0</v>
+        <v>212.3149906599047</v>
       </c>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>65.71641987298243</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
@@ -11372,10 +11372,10 @@
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>10.12574714858493</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>126.0910353404088</v>
       </c>
       <c r="K45" t="n">
         <v>137.841438974359</v>
@@ -11384,10 +11384,10 @@
         <v>138.5543797798742</v>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>142.1340339220183</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>131.3417120833333</v>
       </c>
       <c r="O45" t="n">
         <v>142.5962444444444</v>
@@ -11399,7 +11399,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>45.52166981132082</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
@@ -11454,28 +11454,28 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>33.63624132272333</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>106.7437663446525</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>134.8846762812383</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>138.9257839476051</v>
       </c>
       <c r="N46" t="n">
         <v>127.6855444652332</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>138.4565384518428</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>135.0065633140411</v>
       </c>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>65.34295837775146</v>
       </c>
       <c r="R46" t="n">
         <v>0</v>
@@ -22570,7 +22570,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J2" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -22585,16 +22585,16 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R2" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S2" t="n">
         <v>209.0200695862453</v>
@@ -22646,13 +22646,13 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I3" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J3" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K3" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -22670,10 +22670,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S3" t="n">
         <v>171.6831711038378</v>
@@ -22728,28 +22728,28 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J4" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K4" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L4" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q4" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R4" t="n">
         <v>177.2933913771695</v>
@@ -22807,7 +22807,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J5" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -22822,16 +22822,16 @@
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R5" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S5" t="n">
         <v>209.0200695862453</v>
@@ -22883,16 +22883,16 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I6" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J6" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -22910,7 +22910,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S6" t="n">
         <v>171.6831711038378</v>
@@ -22965,10 +22965,10 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J7" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K7" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -22980,13 +22980,13 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q7" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R7" t="n">
         <v>177.2933913771695</v>
@@ -23044,7 +23044,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J8" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -23059,16 +23059,16 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R8" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S8" t="n">
         <v>209.0200695862453</v>
@@ -23120,34 +23120,34 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I9" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J9" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K9" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S9" t="n">
         <v>171.6831711038378</v>
@@ -23202,10 +23202,10 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J10" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K10" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -23220,10 +23220,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q10" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R10" t="n">
         <v>177.2933913771695</v>
@@ -23281,16 +23281,16 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J11" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -23299,13 +23299,13 @@
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R11" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S11" t="n">
         <v>209.0200695862453</v>
@@ -23357,13 +23357,13 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I12" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J12" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K12" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -23372,19 +23372,19 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S12" t="n">
         <v>171.6831711038378</v>
@@ -23439,28 +23439,28 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J13" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K13" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L13" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q13" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R13" t="n">
         <v>177.2933913771695</v>
@@ -23518,10 +23518,10 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J14" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K14" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
@@ -23530,19 +23530,19 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R14" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S14" t="n">
         <v>209.0200695862453</v>
@@ -23594,10 +23594,10 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I15" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J15" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -23606,22 +23606,22 @@
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S15" t="n">
         <v>171.6831711038378</v>
@@ -23676,16 +23676,16 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J16" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K16" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -23694,10 +23694,10 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q16" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R16" t="n">
         <v>177.2933913771695</v>
@@ -23755,31 +23755,31 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J17" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K17" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R17" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S17" t="n">
         <v>209.0200695862453</v>
@@ -23831,25 +23831,25 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I18" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J18" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K18" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -23858,7 +23858,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S18" t="n">
         <v>171.6831711038378</v>
@@ -23913,28 +23913,28 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J19" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K19" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q19" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R19" t="n">
         <v>177.2933913771695</v>
@@ -23992,31 +23992,31 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J20" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K20" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R20" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S20" t="n">
         <v>209.0200695862453</v>
@@ -24068,22 +24068,22 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I21" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J21" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -24095,7 +24095,7 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S21" t="n">
         <v>171.6831711038378</v>
@@ -24150,10 +24150,10 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J22" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K22" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
@@ -24162,16 +24162,16 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q22" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R22" t="n">
         <v>177.2933913771695</v>
@@ -24229,7 +24229,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J23" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -24244,16 +24244,16 @@
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R23" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S23" t="n">
         <v>209.0200695862453</v>
@@ -24305,22 +24305,22 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I24" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J24" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K24" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
@@ -24332,7 +24332,7 @@
         <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S24" t="n">
         <v>171.6831711038378</v>
@@ -24387,16 +24387,16 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J25" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K25" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L25" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -24405,10 +24405,10 @@
         <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q25" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R25" t="n">
         <v>177.2933913771695</v>
@@ -24466,31 +24466,31 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J26" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K26" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
         <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R26" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S26" t="n">
         <v>209.0200695862453</v>
@@ -24542,16 +24542,16 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I27" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J27" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K27" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
         <v>0</v>
@@ -24560,16 +24560,16 @@
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>142.5962444444444</v>
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S27" t="n">
         <v>171.6831711038378</v>
@@ -24624,13 +24624,13 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J28" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K28" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L28" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
         <v>0</v>
@@ -24639,13 +24639,13 @@
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q28" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R28" t="n">
         <v>177.2933913771695</v>
@@ -24703,31 +24703,31 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J29" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P29" t="n">
         <v>0</v>
       </c>
       <c r="Q29" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R29" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S29" t="n">
         <v>209.0200695862453</v>
@@ -24779,19 +24779,19 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I30" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J30" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K30" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -24800,13 +24800,13 @@
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S30" t="n">
         <v>171.6831711038378</v>
@@ -24861,10 +24861,10 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J31" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K31" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L31" t="n">
         <v>0</v>
@@ -24876,13 +24876,13 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q31" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R31" t="n">
         <v>177.2933913771695</v>
@@ -24940,7 +24940,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J32" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -24958,13 +24958,13 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R32" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S32" t="n">
         <v>209.0200695862453</v>
@@ -25016,19 +25016,19 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I33" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J33" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K33" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
         <v>0</v>
@@ -25037,13 +25037,13 @@
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S33" t="n">
         <v>171.6831711038378</v>
@@ -25098,13 +25098,13 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J34" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K34" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L34" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -25116,10 +25116,10 @@
         <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q34" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R34" t="n">
         <v>177.2933913771695</v>
@@ -25177,7 +25177,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J35" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -25186,22 +25186,22 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q35" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R35" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S35" t="n">
         <v>209.0200695862453</v>
@@ -25253,34 +25253,34 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I36" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J36" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K36" t="n">
-        <v>137.841438974359</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S36" t="n">
         <v>171.6831711038378</v>
@@ -25335,16 +25335,16 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J37" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K37" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L37" t="n">
         <v>0</v>
       </c>
       <c r="M37" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
@@ -25353,10 +25353,10 @@
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q37" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R37" t="n">
         <v>177.2933913771695</v>
@@ -25414,31 +25414,31 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J38" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K38" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L38" t="n">
         <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>230.0982114216867</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
         <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R38" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S38" t="n">
         <v>209.0200695862453</v>
@@ -25490,10 +25490,10 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I39" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J39" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -25514,10 +25514,10 @@
         <v>0</v>
       </c>
       <c r="Q39" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R39" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S39" t="n">
         <v>171.6831711038378</v>
@@ -25572,16 +25572,16 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J40" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K40" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L40" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N40" t="n">
         <v>0</v>
@@ -25590,10 +25590,10 @@
         <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q40" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R40" t="n">
         <v>177.2933913771695</v>
@@ -25651,7 +25651,7 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J41" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
@@ -25660,22 +25660,22 @@
         <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N41" t="n">
-        <v>229.4130635965909</v>
+        <v>0</v>
       </c>
       <c r="O41" t="n">
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R41" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S41" t="n">
         <v>209.0200695862453</v>
@@ -25727,34 +25727,34 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I42" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J42" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>138.5543797798742</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>133.9744074143302</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>139.9817740860215</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S42" t="n">
         <v>171.6831711038378</v>
@@ -25809,10 +25809,10 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J43" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K43" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L43" t="n">
         <v>0</v>
@@ -25821,16 +25821,16 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>127.6855444652332</v>
+        <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P43" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q43" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R43" t="n">
         <v>177.2933913771695</v>
@@ -25888,16 +25888,16 @@
         <v>210.4758895704059</v>
       </c>
       <c r="J44" t="n">
-        <v>181.0459045266863</v>
+        <v>11.94928935461252</v>
       </c>
       <c r="K44" t="n">
-        <v>220.0898510449805</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>235.7664149699872</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>230.3462332272727</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
@@ -25906,13 +25906,13 @@
         <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>231.2329957552695</v>
+        <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>222.3056898744495</v>
+        <v>9.990699214544804</v>
       </c>
       <c r="R44" t="n">
-        <v>215.5855378141321</v>
+        <v>149.8691179411497</v>
       </c>
       <c r="S44" t="n">
         <v>209.0200695862453</v>
@@ -25964,10 +25964,10 @@
         <v>112.2354442364965</v>
       </c>
       <c r="I45" t="n">
-        <v>99.52238</v>
+        <v>89.39663285141508</v>
       </c>
       <c r="J45" t="n">
-        <v>126.8376266666667</v>
+        <v>0.7465913262578567</v>
       </c>
       <c r="K45" t="n">
         <v>0</v>
@@ -25976,10 +25976,10 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>142.1340339220183</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>131.3417120833333</v>
+        <v>0</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -25991,7 +25991,7 @@
         <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>145.679503963964</v>
+        <v>100.1578341526431</v>
       </c>
       <c r="S45" t="n">
         <v>171.6831711038378</v>
@@ -26046,28 +26046,28 @@
         <v>155.4504749272583</v>
       </c>
       <c r="J46" t="n">
-        <v>126.9954214393961</v>
+        <v>93.35918011667277</v>
       </c>
       <c r="K46" t="n">
-        <v>129.0132581705354</v>
+        <v>22.26949182588285</v>
       </c>
       <c r="L46" t="n">
-        <v>134.8846762812383</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>138.9257839476051</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>138.4565384518428</v>
+        <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>137.7280040491476</v>
+        <v>2.721440735106512</v>
       </c>
       <c r="Q46" t="n">
-        <v>151.5050016294458</v>
+        <v>86.16204325169439</v>
       </c>
       <c r="R46" t="n">
         <v>177.2933913771695</v>
@@ -26125,7 +26125,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>216665.3565283203</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="3">
@@ -26133,7 +26133,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>238046.7615399077</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="4">
@@ -26141,7 +26141,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>160164.1557457211</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="5">
@@ -26149,7 +26149,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>142297.6890580523</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="6">
@@ -26157,7 +26157,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>155459.2308154412</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="7">
@@ -26165,7 +26165,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>41901.84325569165</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="8">
@@ -26173,7 +26173,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>117531.0065629728</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="9">
@@ -26181,7 +26181,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>169631.4053910703</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="10">
@@ -26189,7 +26189,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>138886.4814571525</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="11">
@@ -26197,7 +26197,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>152682.9235066417</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="12">
@@ -26205,7 +26205,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>196936.9755371677</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="13">
@@ -26213,7 +26213,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>101470.8883970057</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="14">
@@ -26221,7 +26221,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>169510.2376286328</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="15">
@@ -26229,7 +26229,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>138408.3194632264</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
     <row r="16">
@@ -26237,7 +26237,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>120789.4732342538</v>
+        <v>376275.9193600624</v>
       </c>
     </row>
   </sheetData>
@@ -26521,49 +26521,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-33627.6</v>
+        <v>-48778.27397003476</v>
       </c>
       <c r="C6" t="n">
-        <v>-33627.6</v>
+        <v>-48778.27397003476</v>
       </c>
       <c r="D6" t="n">
-        <v>-33627.6</v>
+        <v>-48778.27397003476</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>-15150.67397003476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>